<commit_message>
readme test case update
</commit_message>
<xml_diff>
--- a/test_case.xlsx
+++ b/test_case.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yixun\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D2DB08D-0E46-4924-A962-FFB60F6E9137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E248C9DC-3267-47AB-B57B-0A55EDD92507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{0FE418D9-40D9-41AF-8F0F-CBBF0FE5BF10}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0FE418D9-40D9-41AF-8F0F-CBBF0FE5BF10}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$21</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$2:$E$23</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t>Test Case #</t>
   </si>
@@ -125,49 +125,63 @@
     <t xml:space="preserve"> Clicking product tab will link user to product page</t>
   </si>
   <si>
+    <t xml:space="preserve">1)Clicking on person icon dropdown after logging in </t>
+  </si>
+  <si>
+    <t>1)Users will see cart item tab , clicking on it will lead to cart item (shoppping cart )page</t>
+  </si>
+  <si>
+    <t>User at Navbar(Orders Page)</t>
+  </si>
+  <si>
+    <t>1)Users will see order tab , clicking on it will lead to order item page</t>
+  </si>
+  <si>
+    <t>User at Navbar(Logout)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)Users will see logout tab </t>
+  </si>
+  <si>
+    <t>1)Upon clicking logout, redirect to homepage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Users able to update the quantity by keying the desired  value in the input field and click on update 
+2) Users are able to delete the cart item by clicking on bin icon located at the  right-middle section of the whole box.Items will then be removed from shopping cart
+3) At the bottom right of the box user able to checkout products, clicking on checkout will lead users to the stripe payment checkout page.Users able to go to shopping page by clicking on continue to shop button located beside checout button
+ </t>
+  </si>
+  <si>
+    <t>1)Users able to see ordered item whether it is pending or completed. Item ordered date ,cost ,status,  quantity ,name, id
+2)Users able to click on more details button to look at the details of the product at details product page. Order address,shipping method,order status, payment method, order id will be shown in the more details page.The back button under order details page  will lead user back to the orders page
+3)The receipt button will lead to receipt page where a summary of product quantity amount charged will be shown</t>
+  </si>
+  <si>
+    <t>User at Navbar (Contact Us Tab)</t>
+  </si>
+  <si>
+    <t>Clicking on contact us tab at navbar</t>
+  </si>
+  <si>
+    <t>Clicking  will link to contact us page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Users are able to fill in contact us page, fields like name, email , types of enquiries and comments.
+2) By clicking on submit black button at the bottom of the contact us box , successfully submitted toaster will show .  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)After user at the register page, users are to fill in their details eg. Name, username, email, password, contact_number
+2) Users are able to click on submit after registering and  it will bring users to login page
+3)Users are to fill in email, password at the login page to access the web product page to make purchase
+*validation error fields for  both login and register page  will show if invalid information is filled and submit
+* after login if users are not active for 60 mins a session will prompt users whether to continue </t>
+  </si>
+  <si>
     <t xml:space="preserve">1) Refer to test Case 3
 *Continue from test Case 3
 2) When users click on products or more button it will bring users to the detail page
 3) The detail page will show more details of the product like shelf- life, type, packaging, cuisine style, cost ,ingredients,country
-4)Users are able to select size,input the quantity and add item to cart by clicking add to cart button. User are able to go back to product page by clicking on back to shop button located at the bottom of page </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1)Clicking on person icon dropdown after logging in </t>
-  </si>
-  <si>
-    <t>1)Users will see cart item tab , clicking on it will lead to cart item (shoppping cart )page</t>
-  </si>
-  <si>
-    <t>1)After user at the register page, users are to fill in their details eg. Name, username, email, password, contact_number
-2) Users are able to click on submit after registering and  it will bring users to login page
-3)Users are to fill in email, password at the login page to access the web to make purchase
-*validation error fields for  both login and register page  will show if invalid information is filled and submit</t>
-  </si>
-  <si>
-    <t>User at Navbar(Orders Page)</t>
-  </si>
-  <si>
-    <t>1)Users will see order tab , clicking on it will lead to order item page</t>
-  </si>
-  <si>
-    <t>User at Navbar(Logout)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1)Users will see logout tab </t>
-  </si>
-  <si>
-    <t>1)Upon clicking logout, redirect to homepage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1) Users able to update the quantity by keying the desired  value in the input field and click on update 
-2) Users are able to delete the cart item by clicking on bin icon located at the  right-middle section of the whole box.Items will then be removed from shopping cart
-3) At the bottom right of the box user able to checkout products, clicking on checkout will lead users to the stripe payment checkout page.Users able to go to shopping page by clicking on continue to shop button located beside checout button
- </t>
-  </si>
-  <si>
-    <t>1)Users able to see ordered item whether it is pending or completed. Item ordered date ,cost ,status,  quantity ,name, id
-2)Users able to click on more details button to look at the details of the product at details product page. Order address,shipping method,order status, payment method, order id will be shown in the more details page.The back button under order details page  will lead user back to the orders page
-3)The receipt button will lead to receipt page where a summary of product quantity amount charged will be shown</t>
+4)Users are able to select size,input the quantity and add item to cart by clicking add to cart button. Users are able to go back to product page by clicking on back to shop button located at the bottom of page </t>
   </si>
 </sst>
 </file>
@@ -228,7 +242,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -251,11 +265,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -280,10 +346,16 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -601,22 +673,22 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E21"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
-    <col min="2" max="2" width="71.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.5546875" customWidth="1"/>
+    <col min="2" max="2" width="71.33203125" customWidth="1"/>
     <col min="3" max="3" width="85" customWidth="1"/>
-    <col min="4" max="4" width="52.42578125" customWidth="1"/>
+    <col min="4" max="4" width="52.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:4" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="7.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:4" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -630,7 +702,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -638,7 +710,7 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -652,7 +724,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
         <v>7</v>
@@ -660,7 +732,7 @@
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>2</v>
       </c>
@@ -674,7 +746,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
         <v>10</v>
@@ -682,7 +754,7 @@
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4" ht="231.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="222.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>3</v>
       </c>
@@ -696,7 +768,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>15</v>
@@ -704,7 +776,7 @@
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:4" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="84.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>4</v>
       </c>
@@ -718,7 +790,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="100.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="5" t="s">
         <v>20</v>
@@ -726,7 +798,7 @@
       <c r="C11" s="1"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" ht="175.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="175.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>5</v>
       </c>
@@ -737,141 +809,163 @@
         <v>21</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="262.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="5" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" spans="1:4" ht="157.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="87.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>6</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="46.15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="68.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-    </row>
-    <row r="16" spans="1:4" ht="202.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" spans="1:4" ht="214.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>7</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
+      <c r="B16" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="12"/>
       <c r="B17" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="6"/>
-    </row>
-    <row r="18" spans="1:4" ht="208.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="C17" s="13"/>
+      <c r="D17" s="5"/>
+    </row>
+    <row r="18" spans="1:4" ht="202.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>8</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="6"/>
     </row>
-    <row r="20" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="208.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>9</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="176.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="9"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="6"/>
+    </row>
+    <row r="22" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>10</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="176.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="10"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="9"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="8"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="8"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="8"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="8"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="8"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="8"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="8"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="8"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="8"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="8"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="8"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="8"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changes to test case and readme
</commit_message>
<xml_diff>
--- a/test_case.xlsx
+++ b/test_case.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yixun\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1FCAF8-EFAD-4ED0-BA4C-671B7FFDCC1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8EDAC45E-DEC6-4B1F-84AA-A3B4355A3A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0FE418D9-40D9-41AF-8F0F-CBBF0FE5BF10}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0FE418D9-40D9-41AF-8F0F-CBBF0FE5BF10}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>